<commit_message>
oke in sha Allah
</commit_message>
<xml_diff>
--- a/rekomendasi.xlsx
+++ b/rekomendasi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,37 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Eu Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Manhattan</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ma Value</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Minkowski</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Mi Value</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Supremum</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Su Value</t>
         </is>
       </c>
     </row>
@@ -463,17 +483,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>4.127953488110059</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Honda City</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>7.2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Honda City</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>4.127953488110059</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Honda City</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3.0</t>
         </is>
       </c>
     </row>
@@ -485,17 +525,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>5.220153254455275</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Toyota Vios</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Toyota Corolla Altis</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5.220153254455275</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Toyota Corolla Altis</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>3.5</t>
         </is>
       </c>
     </row>
@@ -507,17 +567,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>5.477225575051661</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Xpander</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Toyota Vios</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>5.477225575051661</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>Toyota Agya</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>4.0</t>
         </is>
       </c>
     </row>

</xml_diff>